<commit_message>
chore: sync code and remove large assets
</commit_message>
<xml_diff>
--- a/web/public/templates/cases_template.xlsx
+++ b/web/public/templates/cases_template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,10 +419,31 @@
         <v>사진1</v>
       </c>
       <c r="F1" t="str">
+        <v>사진1설명</v>
+      </c>
+      <c r="G1" t="str">
         <v>사진2</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
+        <v>사진2설명</v>
+      </c>
+      <c r="I1" t="str">
         <v>사진3</v>
+      </c>
+      <c r="J1" t="str">
+        <v>사진3설명</v>
+      </c>
+      <c r="K1" t="str">
+        <v>사진4</v>
+      </c>
+      <c r="L1" t="str">
+        <v>사진4설명</v>
+      </c>
+      <c r="M1" t="str">
+        <v>사진5</v>
+      </c>
+      <c r="N1" t="str">
+        <v>사진5설명</v>
       </c>
     </row>
     <row r="2">
@@ -447,6 +468,27 @@
       <c r="G2" t="str">
         <v/>
       </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v/>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -456,10 +498,10 @@
         <v>차대</v>
       </c>
       <c r="C3" t="str">
-        <v>브레이크 레버 유격 과다</v>
+        <v>브레이크 레버 간격 과다</v>
       </c>
       <c r="D3" t="str">
-        <v>레버 유격 조정 후 재점검</v>
+        <v>레버 간격 조정 후 점검</v>
       </c>
       <c r="E3" t="str">
         <v/>
@@ -468,6 +510,27 @@
         <v/>
       </c>
       <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v/>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+      <c r="N3" t="str">
         <v/>
       </c>
     </row>
@@ -479,7 +542,7 @@
         <v>전장</v>
       </c>
       <c r="C4" t="str">
-        <v>시동 후 경고등 점등</v>
+        <v>시동 경고등 점등</v>
       </c>
       <c r="D4" t="str">
         <v>배선 커넥터 접촉 상태 확인</v>
@@ -491,12 +554,33 @@
         <v/>
       </c>
       <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
+        <v/>
+      </c>
+      <c r="L4" t="str">
+        <v/>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+      <c r="N4" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add diagnosis trees DB support and cases extensions
</commit_message>
<xml_diff>
--- a/web/public/templates/cases_template.xlsx
+++ b/web/public/templates/cases_template.xlsx
@@ -397,53 +397,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>차종</v>
+        <v>model</v>
       </c>
       <c r="B1" t="str">
-        <v>고장분류</v>
+        <v>system</v>
       </c>
       <c r="C1" t="str">
-        <v>증상</v>
+        <v>category</v>
       </c>
       <c r="D1" t="str">
-        <v>조치</v>
+        <v>symptomTitle</v>
       </c>
       <c r="E1" t="str">
-        <v>사진1</v>
+        <v>diagnosisTreeId</v>
       </c>
       <c r="F1" t="str">
-        <v>사진1설명</v>
+        <v>diagnosisResultId</v>
       </c>
       <c r="G1" t="str">
-        <v>사진2</v>
+        <v>title</v>
       </c>
       <c r="H1" t="str">
-        <v>사진2설명</v>
+        <v>description</v>
       </c>
       <c r="I1" t="str">
-        <v>사진3</v>
+        <v>fixSteps</v>
       </c>
       <c r="J1" t="str">
-        <v>사진3설명</v>
+        <v>tags</v>
       </c>
       <c r="K1" t="str">
-        <v>사진4</v>
+        <v>references</v>
       </c>
       <c r="L1" t="str">
-        <v>사진4설명</v>
+        <v>parts</v>
       </c>
       <c r="M1" t="str">
-        <v>사진5</v>
+        <v>photo_1</v>
       </c>
       <c r="N1" t="str">
-        <v>사진5설명</v>
+        <v>photo_1_desc</v>
+      </c>
+      <c r="O1" t="str">
+        <v>photo_2</v>
+      </c>
+      <c r="P1" t="str">
+        <v>photo_2_desc</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>photo_3</v>
+      </c>
+      <c r="R1" t="str">
+        <v>photo_3_desc</v>
+      </c>
+      <c r="S1" t="str">
+        <v>photo_4</v>
+      </c>
+      <c r="T1" t="str">
+        <v>photo_4_desc</v>
+      </c>
+      <c r="U1" t="str">
+        <v>photo_5</v>
+      </c>
+      <c r="V1" t="str">
+        <v>photo_5_desc</v>
       </c>
     </row>
     <row r="2">
@@ -451,42 +475,66 @@
         <v>350D</v>
       </c>
       <c r="B2" t="str">
-        <v>엔진</v>
+        <v>engine</v>
       </c>
       <c r="C2" t="str">
-        <v>드레인볼트 토크값 확인 필요</v>
+        <v>Engine</v>
       </c>
       <c r="D2" t="str">
-        <v>매뉴얼 기준 23 N·m로 체결</v>
+        <v>Poor acceleration</v>
       </c>
       <c r="E2" t="str">
-        <v/>
+        <v>poor_acceleration_v1</v>
       </c>
       <c r="F2" t="str">
-        <v/>
+        <v>r3</v>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>Throttle cable free play out of spec</v>
       </c>
       <c r="H2" t="str">
-        <v/>
+        <v>Low acceleration after warm-up</v>
       </c>
       <c r="I2" t="str">
-        <v/>
+        <v>Adjust throttle cable free play to spec</v>
       </c>
       <c r="J2" t="str">
-        <v/>
+        <v>engine,acceleration</v>
       </c>
       <c r="K2" t="str">
-        <v/>
+        <v>https://example.com</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>Throttle cable</v>
       </c>
       <c r="M2" t="str">
         <v/>
       </c>
       <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <v/>
+      </c>
+      <c r="P2" t="str">
+        <v/>
+      </c>
+      <c r="Q2" t="str">
+        <v/>
+      </c>
+      <c r="R2" t="str">
+        <v/>
+      </c>
+      <c r="S2" t="str">
+        <v/>
+      </c>
+      <c r="T2" t="str">
+        <v/>
+      </c>
+      <c r="U2" t="str">
+        <v/>
+      </c>
+      <c r="V2" t="str">
         <v/>
       </c>
     </row>
@@ -495,37 +543,37 @@
         <v>368G</v>
       </c>
       <c r="B3" t="str">
-        <v>차대</v>
+        <v>engine</v>
       </c>
       <c r="C3" t="str">
-        <v>브레이크 레버 간격 과다</v>
+        <v>Idle</v>
       </c>
       <c r="D3" t="str">
-        <v>레버 간격 조정 후 점검</v>
+        <v>High hot idle</v>
       </c>
       <c r="E3" t="str">
-        <v/>
+        <v>high_hot_idle_v1</v>
       </c>
       <c r="F3" t="str">
-        <v/>
+        <v>r4</v>
       </c>
       <c r="G3" t="str">
-        <v/>
+        <v>Coolant temp sensor fault</v>
       </c>
       <c r="H3" t="str">
-        <v/>
+        <v>Idle speed remains high after warm-up</v>
       </c>
       <c r="I3" t="str">
-        <v/>
+        <v>Inspect wiring and replace coolant temperature sensor</v>
       </c>
       <c r="J3" t="str">
-        <v/>
+        <v>idle,sensor</v>
       </c>
       <c r="K3" t="str">
         <v/>
       </c>
       <c r="L3" t="str">
-        <v/>
+        <v>Coolant temperature sensor</v>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -533,54 +581,34 @@
       <c r="N3" t="str">
         <v/>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>125M</v>
-      </c>
-      <c r="B4" t="str">
-        <v>전장</v>
-      </c>
-      <c r="C4" t="str">
-        <v>시동 경고등 점등</v>
-      </c>
-      <c r="D4" t="str">
-        <v>배선 커넥터 접촉 상태 확인</v>
-      </c>
-      <c r="E4" t="str">
-        <v/>
-      </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <v/>
-      </c>
-      <c r="H4" t="str">
-        <v/>
-      </c>
-      <c r="I4" t="str">
-        <v/>
-      </c>
-      <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v/>
-      </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-      <c r="M4" t="str">
-        <v/>
-      </c>
-      <c r="N4" t="str">
+      <c r="O3" t="str">
+        <v/>
+      </c>
+      <c r="P3" t="str">
+        <v/>
+      </c>
+      <c r="Q3" t="str">
+        <v/>
+      </c>
+      <c r="R3" t="str">
+        <v/>
+      </c>
+      <c r="S3" t="str">
+        <v/>
+      </c>
+      <c r="T3" t="str">
+        <v/>
+      </c>
+      <c r="U3" t="str">
+        <v/>
+      </c>
+      <c r="V3" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:V3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>